<commit_message>
original excel files updated
</commit_message>
<xml_diff>
--- a/data/hr_list.xlsx
+++ b/data/hr_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad6921c7f953aa9b/Desktop/New folder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{29A48C08-DC98-4621-BAB2-42D96B6745C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65C76EB7-CD00-4945-8F52-13021B9DFDBB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF30227-B52B-42C8-88BE-2F622C7EB646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{844133E6-C309-4739-A15E-4479D58BCE00}"/>
   </bookViews>
@@ -69,7 +69,7 @@
     <t>Password</t>
   </si>
   <si>
-    <t>123abc</t>
+    <t>Deepchayan@05</t>
   </si>
 </sst>
 </file>
@@ -175,10 +175,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -197,10 +197,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -503,7 +499,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,10 +557,10 @@
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="8"/>
+      <c r="H2" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>